<commit_message>
added XUV spectrometer anuglar accetance spreadsheet again
</commit_message>
<xml_diff>
--- a/XUVSpectrometerTesting/E338XUVWalkingTest_angularAcceptanceMeasurement09212022.xlsx
+++ b/XUVSpectrometerTesting/E338XUVWalkingTest_angularAcceptanceMeasurement09212022.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cemma/Documents/Work/FACET-II/E338/PAX_repo/XUVSpectrometerTesting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63196864-ECEC-AA4C-B597-87877C2BDDEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A97B5E2-8AEB-ED4C-97FA-CA95DAC4F9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="820" windowWidth="27640" windowHeight="16940" xr2:uid="{01D92A44-9A00-8046-B39C-4DBC806BB4A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t xml:space="preserve">Zeroth order centroid [pix] </t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Signal gone</t>
+  </si>
+  <si>
+    <t>Distance from mirror to screen = 113 cm</t>
   </si>
 </sst>
 </file>
@@ -408,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DBCD6E-001B-F14E-B923-F25316A29974}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -425,265 +428,252 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>784</v>
-      </c>
-      <c r="C2">
-        <v>687</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>784</v>
       </c>
       <c r="C3">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="D3">
-        <f>D2+3</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C4">
-        <v>695</v>
+        <v>684</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D8" si="0">D3+3</f>
-        <v>6</v>
+        <f>D3+3</f>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>783</v>
+      </c>
+      <c r="C5">
+        <v>695</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D9" si="0">D4+3</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>781</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>692</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>780</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>693</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>778</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>694</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>779</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>693</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>-1</v>
-      </c>
-      <c r="B9">
-        <v>780</v>
-      </c>
-      <c r="C9">
-        <v>690</v>
-      </c>
-      <c r="D9">
-        <v>-3</v>
-      </c>
-    </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="B10">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="C10">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="D10">
-        <f>D9-3</f>
-        <v>-6</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="B11">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="C11">
         <v>694</v>
       </c>
       <c r="D11">
-        <f t="shared" ref="D11:D13" si="1">D10-3</f>
-        <v>-9</v>
+        <f>D10-3</f>
+        <v>-6</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="B12">
-        <v>774</v>
+        <v>777</v>
       </c>
       <c r="C12">
         <v>694</v>
       </c>
       <c r="D12">
+        <f t="shared" ref="D12:D14" si="1">D11-3</f>
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>-4</v>
+      </c>
+      <c r="B13">
+        <v>774</v>
+      </c>
+      <c r="C13">
+        <v>694</v>
+      </c>
+      <c r="D13">
         <f t="shared" si="1"/>
         <v>-12</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>-5</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>767</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>699</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <f t="shared" si="1"/>
         <v>-15</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>-6</v>
-      </c>
-      <c r="B14">
-        <v>756</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14">
-        <f>D13-3</f>
-        <v>-18</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>7</v>
+        <v>-6</v>
       </c>
       <c r="B15">
-        <v>784</v>
-      </c>
-      <c r="C15">
-        <v>688</v>
+        <v>756</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
       </c>
       <c r="D15">
-        <v>21</v>
+        <f>D14-3</f>
+        <v>-18</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16">
-        <v>792</v>
+        <v>784</v>
       </c>
       <c r="C16">
-        <v>678</v>
+        <v>688</v>
       </c>
       <c r="D16">
-        <f>D15+3</f>
-        <v>24</v>
-      </c>
-      <c r="E16" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17">
-        <v>798</v>
+        <v>792</v>
       </c>
       <c r="C17">
-        <v>669</v>
+        <v>678</v>
       </c>
       <c r="D17">
-        <f t="shared" ref="D17:D18" si="2">D16+3</f>
-        <v>27</v>
+        <f>D16+3</f>
+        <v>24</v>
       </c>
       <c r="E17" t="s">
         <v>6</v>
@@ -691,19 +681,37 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <v>798</v>
+      </c>
+      <c r="C18">
+        <v>669</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ref="D18:D19" si="2">D17+3</f>
+        <v>27</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>10</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>4</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>4</v>
       </c>
-      <c r="D18">
+      <c r="D19">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>